<commit_message>
add: agregado de demo final y actualizacion de md finales
</commit_message>
<xml_diff>
--- a/Entregable-4/Base de datos/productos.xlsx
+++ b/Entregable-4/Base de datos/productos.xlsx
@@ -1,12 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexis Roldan\Box\Proyecto_G25\Entregable-4\Base de datos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34131DAF-2081-439C-94F4-2F50F77150C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="productos.csv" sheetId="1" r:id="rId4"/>
+    <sheet name="productos.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">productos.csv!$C$1:$C$101</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -334,15 +346,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -353,36 +366,43 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -572,20 +592,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,9 +627,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -610,26 +638,26 @@
         <v>5</v>
       </c>
       <c r="D2" s="1">
-        <v>2347.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
-        <v>4973.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>4973</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -638,26 +666,26 @@
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>4964.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>4964</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
-        <v>2033.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -666,26 +694,26 @@
         <v>5</v>
       </c>
       <c r="D6" s="1">
-        <v>4777.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>4777</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4170.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1">
-        <v>7.0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
@@ -694,26 +722,26 @@
         <v>5</v>
       </c>
       <c r="D8" s="1">
-        <v>3269.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>3269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1">
-        <v>4218.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>4218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -722,26 +750,26 @@
         <v>5</v>
       </c>
       <c r="D10" s="1">
-        <v>3878.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>3878</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1">
-        <v>4883.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>4883</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -750,26 +778,26 @@
         <v>5</v>
       </c>
       <c r="D12" s="1">
-        <v>2053.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1">
-        <v>570.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>18</v>
@@ -778,26 +806,26 @@
         <v>5</v>
       </c>
       <c r="D14" s="1">
-        <v>2383.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>2383</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1">
-        <v>1723.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>20</v>
@@ -806,26 +834,26 @@
         <v>5</v>
       </c>
       <c r="D16" s="1">
-        <v>2538.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>2538</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1">
-        <v>4613.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>4613</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
@@ -834,26 +862,26 @@
         <v>5</v>
       </c>
       <c r="D18" s="1">
-        <v>4834.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>4834</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D19" s="1">
-        <v>3444.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>3444</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>24</v>
@@ -862,26 +890,26 @@
         <v>5</v>
       </c>
       <c r="D20" s="1">
-        <v>3251.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>3251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D21" s="1">
-        <v>1571.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>26</v>
@@ -890,26 +918,26 @@
         <v>5</v>
       </c>
       <c r="D22" s="1">
-        <v>272.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D23" s="1">
-        <v>2069.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>28</v>
@@ -918,26 +946,26 @@
         <v>5</v>
       </c>
       <c r="D24" s="1">
-        <v>2380.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1">
-        <v>1305.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>30</v>
@@ -946,26 +974,26 @@
         <v>5</v>
       </c>
       <c r="D26" s="1">
-        <v>4015.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D27" s="1">
-        <v>1001.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>32</v>
@@ -974,26 +1002,26 @@
         <v>5</v>
       </c>
       <c r="D28" s="1">
-        <v>2502.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D29" s="1">
-        <v>936.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>34</v>
@@ -1002,26 +1030,26 @@
         <v>5</v>
       </c>
       <c r="D30" s="1">
-        <v>1868.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D31" s="1">
-        <v>4875.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>4875</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>36</v>
@@ -1030,26 +1058,26 @@
         <v>5</v>
       </c>
       <c r="D32" s="1">
-        <v>3409.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>3409</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D33" s="1">
-        <v>2234.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>38</v>
@@ -1058,26 +1086,26 @@
         <v>5</v>
       </c>
       <c r="D34" s="1">
-        <v>1255.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D35" s="1">
-        <v>503.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>40</v>
@@ -1086,26 +1114,26 @@
         <v>5</v>
       </c>
       <c r="D36" s="1">
-        <v>4430.0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>4430</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D37" s="1">
-        <v>2559.0</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>42</v>
@@ -1114,26 +1142,26 @@
         <v>5</v>
       </c>
       <c r="D38" s="1">
-        <v>3196.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>3196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D39" s="1">
-        <v>1584.0</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>44</v>
@@ -1142,26 +1170,26 @@
         <v>5</v>
       </c>
       <c r="D40" s="1">
-        <v>469.0</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D41" s="1">
-        <v>1215.0</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>46</v>
@@ -1170,26 +1198,26 @@
         <v>5</v>
       </c>
       <c r="D42" s="1">
-        <v>860.0</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D43" s="1">
-        <v>1195.0</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>48</v>
@@ -1198,26 +1226,26 @@
         <v>5</v>
       </c>
       <c r="D44" s="1">
-        <v>887.0</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D45" s="1">
-        <v>2979.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>50</v>
@@ -1226,26 +1254,26 @@
         <v>5</v>
       </c>
       <c r="D46" s="1">
-        <v>745.0</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D47" s="1">
-        <v>3036.0</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>52</v>
@@ -1254,26 +1282,26 @@
         <v>5</v>
       </c>
       <c r="D48" s="1">
-        <v>2939.0</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>2939</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D49" s="1">
-        <v>4462.0</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>4462</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>54</v>
@@ -1282,26 +1310,26 @@
         <v>5</v>
       </c>
       <c r="D50" s="1">
-        <v>2512.0</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>2512</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D51" s="1">
-        <v>727.0</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>56</v>
@@ -1310,12 +1338,12 @@
         <v>5</v>
       </c>
       <c r="D52" s="1">
-        <v>1745.0</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>57</v>
@@ -1324,26 +1352,26 @@
         <v>7</v>
       </c>
       <c r="D53" s="1">
-        <v>2582.0</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D54" s="1">
-        <v>1664.0</v>
-      </c>
-    </row>
-    <row r="55">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>59</v>
@@ -1352,26 +1380,26 @@
         <v>7</v>
       </c>
       <c r="D55" s="1">
-        <v>1592.0</v>
-      </c>
-    </row>
-    <row r="56">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D56" s="1">
-        <v>1407.0</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>61</v>
@@ -1380,40 +1408,40 @@
         <v>7</v>
       </c>
       <c r="D57" s="1">
-        <v>2532.0</v>
-      </c>
-    </row>
-    <row r="58">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D58" s="1">
-        <v>4520.0</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>4520</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D59" s="1">
-        <v>4752.0</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>4752</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>64</v>
@@ -1422,26 +1450,26 @@
         <v>5</v>
       </c>
       <c r="D60" s="1">
-        <v>3612.0</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>3612</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D61" s="1">
-        <v>4647.0</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>4647</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>66</v>
@@ -1450,26 +1478,26 @@
         <v>5</v>
       </c>
       <c r="D62" s="1">
-        <v>4982.0</v>
-      </c>
-    </row>
-    <row r="63">
+        <v>4982</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D63" s="1">
-        <v>3848.0</v>
-      </c>
-    </row>
-    <row r="64">
+        <v>3848</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>68</v>
@@ -1478,26 +1506,26 @@
         <v>5</v>
       </c>
       <c r="D64" s="1">
-        <v>4337.0</v>
-      </c>
-    </row>
-    <row r="65">
+        <v>4337</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D65" s="1">
-        <v>3953.0</v>
-      </c>
-    </row>
-    <row r="66">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>70</v>
@@ -1506,26 +1534,26 @@
         <v>5</v>
       </c>
       <c r="D66" s="1">
-        <v>2423.0</v>
-      </c>
-    </row>
-    <row r="67">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>66.0</v>
+        <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D67" s="1">
-        <v>1533.0</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>67.0</v>
+        <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>72</v>
@@ -1534,26 +1562,26 @@
         <v>5</v>
       </c>
       <c r="D68" s="1">
-        <v>4719.0</v>
-      </c>
-    </row>
-    <row r="69">
+        <v>4719</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D69" s="1">
-        <v>2684.0</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>2684</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>74</v>
@@ -1562,26 +1590,26 @@
         <v>5</v>
       </c>
       <c r="D70" s="1">
-        <v>744.0</v>
-      </c>
-    </row>
-    <row r="71">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D71" s="1">
-        <v>4061.0</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>4061</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>76</v>
@@ -1590,26 +1618,26 @@
         <v>5</v>
       </c>
       <c r="D72" s="1">
-        <v>508.0</v>
-      </c>
-    </row>
-    <row r="73">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D73" s="1">
-        <v>3876.0</v>
-      </c>
-    </row>
-    <row r="74">
+        <v>3876</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>78</v>
@@ -1618,26 +1646,26 @@
         <v>5</v>
       </c>
       <c r="D74" s="1">
-        <v>1561.0</v>
-      </c>
-    </row>
-    <row r="75">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D75" s="1">
-        <v>2953.0</v>
-      </c>
-    </row>
-    <row r="76">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>80</v>
@@ -1646,26 +1674,26 @@
         <v>5</v>
       </c>
       <c r="D76" s="1">
-        <v>3204.0</v>
-      </c>
-    </row>
-    <row r="77">
+        <v>3204</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>76.0</v>
+        <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D77" s="1">
-        <v>4286.0</v>
-      </c>
-    </row>
-    <row r="78">
+        <v>4286</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>82</v>
@@ -1674,26 +1702,26 @@
         <v>5</v>
       </c>
       <c r="D78" s="1">
-        <v>4778.0</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>4778</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D79" s="1">
-        <v>4289.0</v>
-      </c>
-    </row>
-    <row r="80">
+        <v>4289</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>84</v>
@@ -1702,26 +1730,26 @@
         <v>5</v>
       </c>
       <c r="D80" s="1">
-        <v>2420.0</v>
-      </c>
-    </row>
-    <row r="81">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D81" s="1">
-        <v>1981.0</v>
-      </c>
-    </row>
-    <row r="82">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>81.0</v>
+        <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>86</v>
@@ -1730,26 +1758,26 @@
         <v>5</v>
       </c>
       <c r="D82" s="1">
-        <v>2520.0</v>
-      </c>
-    </row>
-    <row r="83">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>82.0</v>
+        <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D83" s="1">
-        <v>2394.0</v>
-      </c>
-    </row>
-    <row r="84">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>88</v>
@@ -1758,26 +1786,26 @@
         <v>5</v>
       </c>
       <c r="D84" s="1">
-        <v>1830.0</v>
-      </c>
-    </row>
-    <row r="85">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D85" s="1">
-        <v>1645.0</v>
-      </c>
-    </row>
-    <row r="86">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>90</v>
@@ -1786,26 +1814,26 @@
         <v>5</v>
       </c>
       <c r="D86" s="1">
-        <v>1856.0</v>
-      </c>
-    </row>
-    <row r="87">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>86.0</v>
+        <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D87" s="1">
-        <v>4090.0</v>
-      </c>
-    </row>
-    <row r="88">
+        <v>4090</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>87.0</v>
+        <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>92</v>
@@ -1814,26 +1842,26 @@
         <v>5</v>
       </c>
       <c r="D88" s="1">
-        <v>1679.0</v>
-      </c>
-    </row>
-    <row r="89">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>88.0</v>
+        <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D89" s="1">
-        <v>2570.0</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>2570</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>89.0</v>
+        <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>94</v>
@@ -1842,12 +1870,12 @@
         <v>5</v>
       </c>
       <c r="D90" s="1">
-        <v>1003.0</v>
-      </c>
-    </row>
-    <row r="91">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>95</v>
@@ -1856,26 +1884,26 @@
         <v>7</v>
       </c>
       <c r="D91" s="1">
-        <v>2902.0</v>
-      </c>
-    </row>
-    <row r="92">
+        <v>2902</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>91.0</v>
+        <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D92" s="1">
-        <v>4690.0</v>
-      </c>
-    </row>
-    <row r="93">
+        <v>4690</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>92.0</v>
+        <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>97</v>
@@ -1884,26 +1912,26 @@
         <v>7</v>
       </c>
       <c r="D93" s="1">
-        <v>2512.0</v>
-      </c>
-    </row>
-    <row r="94">
+        <v>2512</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>93.0</v>
+        <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D94" s="1">
-        <v>2142.0</v>
-      </c>
-    </row>
-    <row r="95">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>99</v>
@@ -1912,26 +1940,26 @@
         <v>7</v>
       </c>
       <c r="D95" s="1">
-        <v>1418.0</v>
-      </c>
-    </row>
-    <row r="96">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>95.0</v>
+        <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D96" s="1">
-        <v>1581.0</v>
-      </c>
-    </row>
-    <row r="97">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>101</v>
@@ -1940,26 +1968,26 @@
         <v>7</v>
       </c>
       <c r="D97" s="1">
-        <v>4920.0</v>
-      </c>
-    </row>
-    <row r="98">
+        <v>4920</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D98" s="1">
-        <v>872.0</v>
-      </c>
-    </row>
-    <row r="99">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>103</v>
@@ -1968,26 +1996,26 @@
         <v>7</v>
       </c>
       <c r="D99" s="1">
-        <v>2843.0</v>
-      </c>
-    </row>
-    <row r="100">
+        <v>2843</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D100" s="1">
-        <v>2430.0</v>
-      </c>
-    </row>
-    <row r="101">
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>105</v>
@@ -1996,10 +2024,11 @@
         <v>7</v>
       </c>
       <c r="D101" s="1">
-        <v>4854.0</v>
+        <v>4854</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <autoFilter ref="C1:C101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>